<commit_message>
Try changing .xls props, add some tests
</commit_message>
<xml_diff>
--- a/test/list.xlsx
+++ b/test/list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dante\Desktop\dates\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\60-ampri\dates\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64C9638-5B82-4642-89DB-351EAA98B70C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312D8ABA-7E3F-4CBD-9F19-65E5ADA94275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28080" windowHeight="17940" xr2:uid="{34D9E79F-F477-472A-9221-F5BC05282977}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="List" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">List!$A$3:$F$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">List!$A$3:$F$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>test.xlsx</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>Path</t>
+  </si>
+  <si>
+    <t>test.xls</t>
   </si>
 </sst>
 </file>
@@ -1027,11 +1030,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1166,28 +1169,53 @@
         <v>38477</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="41" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="34"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="9">
+        <v>36892</v>
+      </c>
+      <c r="H6" s="10">
+        <v>37289</v>
+      </c>
+      <c r="I6" s="8">
+        <v>37683</v>
+      </c>
+      <c r="J6" s="6">
+        <v>38081</v>
+      </c>
+      <c r="K6" s="10">
+        <v>38477</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="28">
+      <c r="B7" s="35"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="28">
         <v>36892</v>
       </c>
-      <c r="H6" s="31">
+      <c r="H7" s="31">
         <v>37289</v>
       </c>
-      <c r="I6" s="21">
+      <c r="I7" s="21">
         <v>37683</v>
       </c>
-      <c r="J6" s="22">
+      <c r="J7" s="22">
         <v>38081</v>
       </c>
-      <c r="K6" s="31">
+      <c r="K7" s="31">
         <v>38477</v>
       </c>
     </row>

</xml_diff>